<commit_message>
Add contributionDescription and remove previous scripts
</commit_message>
<xml_diff>
--- a/prisma/seeds/pwcat.xlsx
+++ b/prisma/seeds/pwcat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36870" windowHeight="14670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33195" windowHeight="14670"/>
   </bookViews>
   <sheets>
     <sheet name="Moons Descriptions and Pictures" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>https://i.imgur.com/NcDIyeJ.png</t>
-  </si>
-  <si>
-    <t>Developer Tools - Nodes &amp; Security</t>
   </si>
   <si>
     <t>In the world of blockchain development, nodes are fundamental. They represent individual points in the network, ensuring data integrity, verification, and transmission. Security, on the other hand, is paramount. With the decentralized nature of blockchain, ensuring that data is secure and immune to malicious attacks is vital. Developer tools in these areas provide the necessary infrastructure, monitoring capabilities, and protective measures to ensure the robustness and safety of the blockchain network.</t>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>pid</t>
+  </si>
+  <si>
+    <t>Explorers, Security &amp; Node Deployment Tools</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -823,13 +823,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -837,13 +837,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -851,13 +851,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -865,13 +865,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -879,13 +879,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -893,13 +893,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -907,13 +907,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -921,13 +921,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -935,13 +935,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -949,13 +949,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -963,13 +963,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -977,13 +977,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -991,13 +991,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3994,24 +3994,24 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="6"/>
@@ -4021,32 +4021,32 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="12" t="s">
+      <c r="B6" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C6" s="12"/>
     </row>
@@ -7075,22 +7075,22 @@
     <row r="1" spans="1:24">
       <c r="A1" s="6"/>
       <c r="B1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="10">
         <f>SUM(B4:B1000)</f>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="10">
         <f>SUM(E4:E1000)</f>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="10">
         <f>SUM(H4:H1000)</f>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2" s="10">
         <f>SUM(K4:K1000)</f>
@@ -7180,28 +7180,28 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="10">
         <v>18</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="10">
         <v>18</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="10">
         <v>20</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K4" s="10">
         <v>19</v>
@@ -7222,28 +7222,28 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10">
         <v>25</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="10">
         <v>20</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="10">
         <v>22</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K5" s="10">
         <v>29</v>
@@ -7264,28 +7264,28 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="10">
         <v>30</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="10">
         <v>21</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" s="10">
         <v>23</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K6" s="10">
         <v>30</v>
@@ -7306,28 +7306,28 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="10">
         <v>31</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="10">
         <v>24</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="10">
         <v>30</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K7" s="10">
         <v>33</v>
@@ -7348,28 +7348,28 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="10">
         <v>32</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="10">
         <v>28</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" s="10">
         <v>34</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K8" s="10">
         <v>31</v>
@@ -7390,14 +7390,14 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="10">
         <v>36</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="10">
         <v>28</v>

</xml_diff>

<commit_message>
Add metadata url to the schema
</commit_message>
<xml_diff>
--- a/prisma/seeds/pwcat.xlsx
+++ b/prisma/seeds/pwcat.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -218,9 +218,6 @@
     <t>https://i.imgur.com/Cb9LcUp.png</t>
   </si>
   <si>
-    <t>Ethereum Infrastructure</t>
-  </si>
-  <si>
     <t>Ethereum Infrastructure refers to the foundational technologies and systems that support the Ethereum blockchain's operation and growth. This includes nodes, consensus mechanisms, smart contract platforms, layer-2 scaling solutions, and more. A robust and scalable infrastructure ensures that Ethereum remains secure, decentralized, and capable of handling a growing number of transactions and applications. As the Ethereum ecosystem continues to evolve, continuous investments in infrastructure development are vital to maintain its position as a leading decentralized platform.</t>
   </si>
   <si>
@@ -347,6 +344,33 @@
   </si>
   <si>
     <t>Explorers, Security &amp; Node Deployment Tools</t>
+  </si>
+  <si>
+    <t>Ethereum Core Tech Foundations</t>
+  </si>
+  <si>
+    <t>International &amp; Multilingual Support</t>
+  </si>
+  <si>
+    <t>Content Creation &amp; Media</t>
+  </si>
+  <si>
+    <t>Governance Tokenomics and Analytics</t>
+  </si>
+  <si>
+    <t>Security &amp; Cross-Chain Solutions</t>
+  </si>
+  <si>
+    <t>User Experience &amp; Adoption</t>
+  </si>
+  <si>
+    <t>Blockchain Education</t>
+  </si>
+  <si>
+    <t>NFTs</t>
+  </si>
+  <si>
+    <t>Development &amp; Infrastructure</t>
   </si>
 </sst>
 </file>
@@ -668,10 +692,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -692,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -823,7 +847,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>30</v>
@@ -991,41 +1015,105 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="5"/>
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" s="5"/>
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="B26" s="5"/>
+      <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="B27" s="5"/>
+      <c r="A27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="5"/>
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="5"/>
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="B30" s="5"/>
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" s="5"/>
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="5"/>
@@ -3930,9 +4018,6 @@
     </row>
     <row r="999" spans="2:2">
       <c r="B999" s="5"/>
-    </row>
-    <row r="1000" spans="2:2">
-      <c r="B1000" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3994,24 +4079,24 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="6"/>
@@ -4021,32 +4106,32 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="12" t="s">
+      <c r="B6" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C6" s="12"/>
     </row>
@@ -7075,22 +7160,22 @@
     <row r="1" spans="1:24">
       <c r="A1" s="6"/>
       <c r="B1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -7108,7 +7193,7 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="10">
         <f>SUM(B4:B1000)</f>
@@ -7116,7 +7201,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="10">
         <f>SUM(E4:E1000)</f>
@@ -7124,7 +7209,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="10">
         <f>SUM(H4:H1000)</f>
@@ -7132,7 +7217,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="10">
         <f>SUM(K4:K1000)</f>
@@ -7180,28 +7265,28 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10">
         <v>18</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="10">
         <v>18</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="10">
         <v>20</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" s="10">
         <v>19</v>
@@ -7222,28 +7307,28 @@
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10">
         <v>25</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="10">
         <v>20</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="10">
         <v>22</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K5" s="10">
         <v>29</v>
@@ -7264,28 +7349,28 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="10">
         <v>30</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="10">
         <v>21</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="10">
         <v>23</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K6" s="10">
         <v>30</v>
@@ -7306,28 +7391,28 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="10">
         <v>31</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" s="10">
         <v>24</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="10">
         <v>30</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K7" s="10">
         <v>33</v>
@@ -7348,28 +7433,28 @@
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="10">
         <v>32</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="10">
         <v>28</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="10">
         <v>34</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K8" s="10">
         <v>31</v>
@@ -7390,14 +7475,14 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="10">
         <v>36</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9" s="10">
         <v>28</v>

</xml_diff>

<commit_message>
A host of mostly naming changes
</commit_message>
<xml_diff>
--- a/prisma/seeds/pwcat.xlsx
+++ b/prisma/seeds/pwcat.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -372,6 +372,9 @@
   <si>
     <t>Development &amp; Infrastructure</t>
   </si>
+  <si>
+    <t>Community Building Projects</t>
+  </si>
 </sst>
 </file>
 
@@ -695,7 +698,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1001,7 +1004,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>63</v>
@@ -1116,7 +1119,16 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="5"/>
+      <c r="A32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="5"/>
@@ -7144,11 +7156,13 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" customWidth="1"/>

</xml_diff>